<commit_message>
Add patients in fake_dataset
</commit_message>
<xml_diff>
--- a/examples/data/fake_dataset.xlsx
+++ b/examples/data/fake_dataset.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxen\Documents\GitHub\ProstateCancerNomograms\examples\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Labo\Documents\GitHub\ProstateCancerNomograms\examples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAD7E6D-39D2-4F4D-9DF3-F943EF6732A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8E1A29-6848-4645-ACCD-F0F1F4384E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,29 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
-  <si>
-    <t>Récurrence 10 ans (120 mois), oui = 1; non =0</t>
-  </si>
-  <si>
-    <t>pN</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>T3a</t>
   </si>
   <si>
-    <t>pN1</t>
-  </si>
-  <si>
     <t>T1-T2</t>
   </si>
   <si>
     <t>T1c</t>
   </si>
   <si>
-    <t>pN0</t>
-  </si>
-  <si>
     <t>T3b</t>
   </si>
   <si>
@@ -88,6 +76,45 @@
   </si>
   <si>
     <t>BCR</t>
+  </si>
+  <si>
+    <t>BCR_TIME</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>SVI</t>
+  </si>
+  <si>
+    <t>METASTASIS</t>
+  </si>
+  <si>
+    <t>METASTASIS_TIME</t>
+  </si>
+  <si>
+    <t>CRPC</t>
+  </si>
+  <si>
+    <t>CRPC_TIME</t>
+  </si>
+  <si>
+    <t>DEATH</t>
+  </si>
+  <si>
+    <t>DEATH_TIME</t>
+  </si>
+  <si>
+    <t>Patient088</t>
+  </si>
+  <si>
+    <t>Patient095</t>
+  </si>
+  <si>
+    <t>Patient102</t>
   </si>
 </sst>
 </file>
@@ -405,183 +432,466 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="22.42578125" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="5.42578125" customWidth="1"/>
+    <col min="13" max="13" width="4.28515625" customWidth="1"/>
+    <col min="14" max="14" width="6" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="6.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>62</v>
+      </c>
+      <c r="D2">
+        <v>1.2</v>
+      </c>
+      <c r="E2">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>62</v>
-      </c>
-      <c r="E2">
-        <v>1.2</v>
-      </c>
       <c r="F2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G2">
         <v>4</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>100</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>100</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>72</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
         <v>4</v>
       </c>
-      <c r="I2" t="s">
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>50</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>70</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>150</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>57</v>
+      </c>
+      <c r="D4">
+        <v>5.5</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
         <v>2</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>120</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>140</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>140</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>66</v>
+      </c>
+      <c r="D5">
+        <v>7.2</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>30</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>150</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>60</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>55</v>
+      </c>
+      <c r="D6">
+        <v>6.7</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
         <v>2</v>
       </c>
-      <c r="M2" t="s">
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>20</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>40</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>120</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>68</v>
+      </c>
+      <c r="D7">
+        <v>12.3</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>72</v>
-      </c>
-      <c r="E3">
-        <v>12</v>
-      </c>
-      <c r="F3">
-        <v>9</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="I7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>57</v>
-      </c>
-      <c r="E4">
-        <v>5.5</v>
-      </c>
-      <c r="F4">
-        <v>9</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>4</v>
-      </c>
-      <c r="I4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M4" t="s">
-        <v>6</v>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>90</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>60</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>100</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add organ confined disease column
</commit_message>
<xml_diff>
--- a/examples/data/fake_dataset.xlsx
+++ b/examples/data/fake_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Labo\Documents\GitHub\ProstateCancerNomograms\examples\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxen\Documents\GitHub\ProstateCancerNomograms\examples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8E1A29-6848-4645-ACCD-F0F1F4384E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182E5FDD-D68D-4B6F-8157-3817E6F6111A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>T3a</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Patient102</t>
+  </si>
+  <si>
+    <t>OCD</t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,18 +452,19 @@
     <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="22.42578125" customWidth="1"/>
     <col min="10" max="10" width="5.28515625" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
     <col min="12" max="12" width="5.42578125" customWidth="1"/>
     <col min="13" max="13" width="4.28515625" customWidth="1"/>
-    <col min="14" max="14" width="6" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" customWidth="1"/>
-    <col min="19" max="19" width="6.7109375" customWidth="1"/>
-    <col min="20" max="20" width="12.28515625" customWidth="1"/>
+    <col min="14" max="15" width="6" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" customWidth="1"/>
+    <col min="18" max="18" width="5.7109375" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" customWidth="1"/>
+    <col min="20" max="20" width="6.7109375" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -504,25 +508,28 @@
         <v>20</v>
       </c>
       <c r="O1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>25</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -569,22 +576,25 @@
         <v>0</v>
       </c>
       <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
         <v>100</v>
       </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
       <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
         <v>100</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
       <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -631,22 +641,25 @@
         <v>1</v>
       </c>
       <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
         <v>70</v>
       </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
       <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
         <v>150</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
       <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -690,25 +703,28 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
         <v>140</v>
       </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
       <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
         <v>140</v>
       </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
       <c r="T4">
-        <v>200</v>
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -752,25 +768,28 @@
         <v>1</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
         <v>150</v>
       </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
       <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
         <v>60</v>
       </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
       <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -817,22 +836,25 @@
         <v>0</v>
       </c>
       <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
         <v>40</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
       <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
         <v>120</v>
       </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
       <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -876,21 +898,24 @@
         <v>1</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
         <v>60</v>
       </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
       <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
         <v>100</v>
       </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
       <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Separate capra and mskcc clinical stage
</commit_message>
<xml_diff>
--- a/examples/data/fake_dataset.xlsx
+++ b/examples/data/fake_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxen\Documents\GitHub\ProstateCancerNomograms\examples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182E5FDD-D68D-4B6F-8157-3817E6F6111A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE7F833-9C4E-4407-A281-5E3DC60D3C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>GLEASON_SECONDARY</t>
   </si>
   <si>
-    <t>CLINICAL_STAGE_CAPRA</t>
-  </si>
-  <si>
     <t>CLINICAL_STAGE</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>OCD</t>
+  </si>
+  <si>
+    <t>CLINICAL_STAGE_MSKCC</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,10 +466,10 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -490,48 +490,48 @@
         <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
-      </c>
-      <c r="U1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -726,7 +726,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -856,7 +856,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7">
         <v>0</v>

</xml_diff>